<commit_message>
Add parsing categories names
</commit_message>
<xml_diff>
--- a/export_data/my_book.xlsx
+++ b/export_data/my_book.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Category id</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -472,8 +472,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>7</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>category 7</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -500,8 +502,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>2</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>category 2</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -528,8 +532,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>8</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>category 8</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -556,8 +562,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>9</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>category 9</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -584,8 +592,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>9</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>category 9</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -612,8 +622,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>category 1</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -640,8 +652,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>6</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>category 6</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -668,8 +682,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>4</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>category 4</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -696,8 +712,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>8</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>category 8</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -724,8 +742,10 @@
           <t>rub</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>9</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>category 9</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add exporting operations for the period
</commit_message>
<xml_diff>
--- a/export_data/my_book.xlsx
+++ b/export_data/my_book.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,16 +486,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>29.12.2020 21:09</t>
+          <t>01.12.2021 00:09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>927</v>
+        <v>467</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -504,7 +504,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>category 2</t>
+          <t>category 8</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -516,16 +516,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01.12.2021 00:09</t>
+          <t>05.05.2021 21:09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>467</v>
+        <v>779</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>category 8</t>
+          <t>category 9</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -546,7 +546,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>05.05.2021 21:09</t>
+          <t>29.12.2021 21:09</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>779</v>
+        <v>205</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -576,16 +576,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>29.12.2021 21:09</t>
+          <t>08.06.2021 21:09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -594,7 +594,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>category 9</t>
+          <t>category 4</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -606,7 +606,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15.12.2019 21:09</t>
+          <t>20.03.2021 16:09</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>917</v>
+        <v>693</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -624,130 +624,10 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>category 1</t>
+          <t>category 9</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>11.11.2020 18:15</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>130</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>rub</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>category 6</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>08.06.2021 21:09</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>228</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>rub</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>category 4</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>27.08.2015 21:09</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>698</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>rub</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>category 8</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>20.03.2021 16:09</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>693</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>rub</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>category 9</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>